<commit_message>
Establecer que solo se envie un archivo y mejor logica
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -5445,7 +5445,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>No se detecta ninguna emoción en el texto</t>
+          <t>negativa</t>
         </is>
       </c>
     </row>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>No se detecta ninguna emoción en el texto</t>
+          <t>negativa</t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>No se detecta ninguna emoción en el texto</t>
+          <t>negativa</t>
         </is>
       </c>
     </row>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>No se detecta ninguna emoción en el texto</t>
+          <t>negativa</t>
         </is>
       </c>
     </row>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>No se detecta ninguna emoción en el texto</t>
+          <t>negativa</t>
         </is>
       </c>
     </row>

</xml_diff>